<commit_message>
Add updates to plan
</commit_message>
<xml_diff>
--- a/Proj 3 Plan.xlsx
+++ b/Proj 3 Plan.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="251">
   <si>
     <t>Technical Requirements</t>
   </si>
@@ -639,9 +639,6 @@
     <t>set up mongodb files</t>
   </si>
   <si>
-    <t>curl requests</t>
-  </si>
-  <si>
     <t>curl create</t>
   </si>
   <si>
@@ -900,9 +897,6 @@
     <t>decide MVP</t>
   </si>
   <si>
-    <t>meeting tonight 6-8 @ Lisa's</t>
-  </si>
-  <si>
     <t>review bootstrap templates</t>
   </si>
   <si>
@@ -991,6 +985,36 @@
   </si>
   <si>
     <t>Open, artifacts attached</t>
+  </si>
+  <si>
+    <t>curl requests client to api</t>
+  </si>
+  <si>
+    <t>donsignin</t>
+  </si>
+  <si>
+    <t>meeting tonight 6-8 @ Don's</t>
+  </si>
+  <si>
+    <t>scripts/auth/api, events, js</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>one of us</t>
+  </si>
+  <si>
+    <t>test sign up from UI</t>
+  </si>
+  <si>
+    <t>test sign out from UI</t>
+  </si>
+  <si>
+    <t>test sign in from UI</t>
+  </si>
+  <si>
+    <t>test change password from UI</t>
   </si>
 </sst>
 </file>
@@ -2016,10 +2040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2043,7 +2067,7 @@
         <v>78</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
@@ -2061,7 +2085,7 @@
         <v>91</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
@@ -2079,7 +2103,7 @@
         <v>92</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
@@ -2209,7 +2233,7 @@
         <v>111</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I12" s="44" t="s">
         <v>101</v>
@@ -2220,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39" t="s">
@@ -2230,11 +2254,11 @@
         <v>42870</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G13" s="40"/>
       <c r="H13" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I13" s="41"/>
     </row>
@@ -2243,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27" t="s">
@@ -2253,14 +2277,14 @@
         <v>42870</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -2268,7 +2292,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27" t="s">
@@ -2278,11 +2302,11 @@
         <v>42870</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I15" s="32"/>
     </row>
@@ -2291,7 +2315,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27" t="s">
@@ -2301,11 +2325,11 @@
         <v>42870</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I16" s="32"/>
     </row>
@@ -2314,7 +2338,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27" t="s">
@@ -2324,11 +2348,11 @@
         <v>42870</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I17" s="32"/>
       <c r="L17" s="17"/>
@@ -2338,7 +2362,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27" t="s">
@@ -2348,11 +2372,11 @@
         <v>42870</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G18" s="27"/>
       <c r="H18" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I18" s="32"/>
     </row>
@@ -2361,7 +2385,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="27" t="s">
@@ -2371,13 +2395,13 @@
         <v>42870</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I19" s="32"/>
     </row>
@@ -2398,10 +2422,10 @@
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I20" s="32" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -2421,10 +2445,10 @@
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
       <c r="H21" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -2442,11 +2466,11 @@
         <v>42870</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I22" s="32"/>
     </row>
@@ -2465,11 +2489,11 @@
         <v>42870</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I23" s="32"/>
     </row>
@@ -2488,11 +2512,11 @@
         <v>42870</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I24" s="32"/>
     </row>
@@ -2501,7 +2525,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="27" t="s">
@@ -2511,11 +2535,11 @@
         <v>42870</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G25" s="28"/>
       <c r="H25" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I25" s="32"/>
     </row>
@@ -2524,7 +2548,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27" t="s">
@@ -2534,11 +2558,11 @@
         <v>42870</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G26" s="27"/>
       <c r="H26" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I26" s="32"/>
     </row>
@@ -2547,7 +2571,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>125</v>
+        <v>241</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27" t="s">
@@ -2605,7 +2629,7 @@
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D30" s="27" t="s">
         <v>83</v>
@@ -2624,7 +2648,7 @@
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D31" s="27" t="s">
         <v>83</v>
@@ -2643,7 +2667,7 @@
       </c>
       <c r="B32" s="27"/>
       <c r="C32" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D32" s="27" t="s">
         <v>83</v>
@@ -2656,12 +2680,12 @@
       <c r="H32" s="27"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="31">
         <v>20</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="27" t="s">
@@ -2670,25 +2694,52 @@
       <c r="E33" s="28">
         <v>42870</v>
       </c>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
+      <c r="F33" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="G33" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="16" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="16" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="27"/>
+      <c r="B34" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="I34" s="27"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="31"/>
+      <c r="B37" s="16" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="31"/>
-      <c r="B37" s="27" t="s">
-        <v>231</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="27" t="s">
@@ -2698,19 +2749,19 @@
         <v>42870</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G37" s="27"/>
       <c r="H37" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="27" t="s">
+        <v>210</v>
       </c>
       <c r="D38" s="27" t="s">
         <v>83</v>
@@ -2718,11 +2769,17 @@
       <c r="E38" s="28">
         <v>42870</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F38" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
       <c r="B39" s="27" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="27" t="s">
@@ -2736,10 +2793,10 @@
       <c r="H39" s="27"/>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="31"/>
       <c r="B40" s="27" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="27" t="s">
@@ -2748,18 +2805,22 @@
       <c r="E40" s="28">
         <v>42870</v>
       </c>
-      <c r="F40" s="27"/>
+      <c r="F40" s="27" t="s">
+        <v>207</v>
+      </c>
       <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
+      <c r="H40" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="31"/>
       <c r="B41" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="27" t="s">
         <v>196</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>197</v>
       </c>
       <c r="D41" s="27" t="s">
         <v>82</v>
@@ -2772,11 +2833,9 @@
       <c r="H41" s="27"/>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="31"/>
-      <c r="B42" s="27" t="s">
-        <v>124</v>
-      </c>
+      <c r="B42" s="27"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27" t="s">
         <v>82</v>
@@ -2789,7 +2848,7 @@
       <c r="H42" s="27"/>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="31"/>
       <c r="B43" s="27"/>
       <c r="C43" s="27" t="s">
@@ -2805,10 +2864,10 @@
       <c r="G43" s="28"/>
       <c r="H43" s="27"/>
       <c r="I43" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="31"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27" t="s">
@@ -2825,9 +2884,11 @@
       <c r="H44" s="27"/>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="31"/>
-      <c r="B45" s="27"/>
+      <c r="B45" s="27" t="s">
+        <v>135</v>
+      </c>
       <c r="C45" s="27" t="s">
         <v>121</v>
       </c>
@@ -2842,10 +2903,10 @@
       <c r="H45" s="27"/>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="31"/>
       <c r="B46" s="27" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27" t="s">
@@ -2859,7 +2920,7 @@
       <c r="H46" s="27"/>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="31"/>
       <c r="B47" s="27" t="s">
         <v>129</v>
@@ -2876,23 +2937,30 @@
       <c r="H47" s="27"/>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="31"/>
       <c r="B48" s="27" t="s">
         <v>130</v>
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E48" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F48" s="27"/>
+        <v>42870</v>
+      </c>
+      <c r="F48" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
+      <c r="H48" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I48" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -2902,16 +2970,20 @@
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E49" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F49" s="27"/>
+        <v>42870</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
+      <c r="H49" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I49" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -2921,35 +2993,43 @@
       </c>
       <c r="C50" s="27"/>
       <c r="D50" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E50" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F50" s="28"/>
+        <v>42870</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G50" s="28"/>
-      <c r="H50" s="27"/>
+      <c r="H50" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I50" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="31"/>
       <c r="B51" s="27" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C51" s="27"/>
       <c r="D51" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E51" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F51" s="27"/>
+        <v>42870</v>
+      </c>
+      <c r="F51" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
+      <c r="H51" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I51" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -2959,16 +3039,20 @@
       </c>
       <c r="C52" s="27"/>
       <c r="D52" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E52" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F52" s="28"/>
+        <v>42870</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G52" s="28"/>
-      <c r="H52" s="27"/>
+      <c r="H52" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I52" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -2978,16 +3062,20 @@
       </c>
       <c r="C53" s="27"/>
       <c r="D53" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E53" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F53" s="28"/>
+        <v>42870</v>
+      </c>
+      <c r="F53" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G53" s="28"/>
-      <c r="H53" s="27"/>
+      <c r="H53" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I53" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -2997,16 +3085,20 @@
       </c>
       <c r="C54" s="27"/>
       <c r="D54" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E54" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F54" s="28"/>
+        <v>42870</v>
+      </c>
+      <c r="F54" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G54" s="28"/>
-      <c r="H54" s="27"/>
+      <c r="H54" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I54" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -3016,16 +3108,20 @@
       </c>
       <c r="C55" s="27"/>
       <c r="D55" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E55" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F55" s="28"/>
+        <v>42870</v>
+      </c>
+      <c r="F55" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G55" s="28"/>
-      <c r="H55" s="27"/>
+      <c r="H55" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I55" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -3035,16 +3131,20 @@
       </c>
       <c r="C56" s="27"/>
       <c r="D56" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E56" s="28">
-        <v>42871</v>
-      </c>
-      <c r="F56" s="28"/>
+        <v>42870</v>
+      </c>
+      <c r="F56" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G56" s="28"/>
-      <c r="H56" s="27"/>
+      <c r="H56" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I56" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -3053,17 +3153,21 @@
         <v>146</v>
       </c>
       <c r="C57" s="27"/>
-      <c r="D57" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E57" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F57" s="28"/>
+      <c r="D57" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F57" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G57" s="28"/>
-      <c r="H57" s="27"/>
+      <c r="H57" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I57" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -3072,397 +3176,451 @@
         <v>147</v>
       </c>
       <c r="C58" s="27"/>
-      <c r="D58" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E58" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F58" s="28"/>
+      <c r="D58" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E58" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F58" s="27" t="s">
+        <v>245</v>
+      </c>
       <c r="G58" s="28"/>
-      <c r="H58" s="27"/>
+      <c r="H58" s="27" t="s">
+        <v>193</v>
+      </c>
       <c r="I58" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="31"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="27" t="s">
-        <v>148</v>
+        <v>247</v>
       </c>
       <c r="C59" s="27"/>
-      <c r="D59" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E59" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
+      <c r="D59" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
       <c r="H59" s="27"/>
-      <c r="I59" s="32" t="s">
-        <v>221</v>
-      </c>
+      <c r="I59" s="27"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="31"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="27" t="s">
-        <v>135</v>
+        <v>249</v>
       </c>
       <c r="C60" s="27"/>
       <c r="D60" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E60" s="28">
         <v>42870</v>
       </c>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
       <c r="H60" s="27"/>
-      <c r="I60" s="32"/>
+      <c r="I60" s="27"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="31"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="27" t="s">
-        <v>137</v>
+        <v>248</v>
       </c>
       <c r="C61" s="27"/>
       <c r="D61" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E61" s="28">
         <v>42870</v>
       </c>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
       <c r="H61" s="27"/>
-      <c r="I61" s="32"/>
+      <c r="I61" s="27"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="31"/>
+      <c r="A62" s="27"/>
       <c r="B62" s="27" t="s">
-        <v>138</v>
+        <v>250</v>
       </c>
       <c r="C62" s="27"/>
       <c r="D62" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E62" s="28">
         <v>42870</v>
       </c>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="27"/>
       <c r="H62" s="27"/>
-      <c r="I62" s="32"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="31"/>
-      <c r="B63" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="E63" s="28">
-        <v>42870</v>
-      </c>
-      <c r="F63" s="28"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="27"/>
-      <c r="I63" s="32"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="31"/>
-      <c r="B64" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="E64" s="28">
-        <v>42870</v>
-      </c>
-      <c r="F64" s="28"/>
-      <c r="G64" s="28"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="32"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="31"/>
-      <c r="B65" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="27"/>
-      <c r="D65" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E65" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F65" s="28"/>
-      <c r="G65" s="28"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="32"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="31"/>
-      <c r="B66" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="C66" s="27"/>
-      <c r="D66" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E66" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F66" s="28"/>
-      <c r="G66" s="28"/>
-      <c r="H66" s="27"/>
-      <c r="I66" s="32"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="31"/>
-      <c r="B67" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C67" s="27"/>
-      <c r="D67" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E67" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F67" s="28"/>
-      <c r="G67" s="28"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="32"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="31"/>
-      <c r="B68" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E68" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F68" s="30"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="32"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="31"/>
-      <c r="B69" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C69" s="29"/>
-      <c r="D69" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E69" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F69" s="30"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="29"/>
-      <c r="I69" s="32"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="31"/>
-      <c r="B70" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C70" s="29"/>
-      <c r="D70" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E70" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F70" s="30"/>
-      <c r="G70" s="30"/>
-      <c r="H70" s="29"/>
-      <c r="I70" s="32"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="31"/>
-      <c r="B71" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C71" s="29"/>
-      <c r="D71" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E71" s="30">
-        <v>42871</v>
-      </c>
-      <c r="F71" s="30"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="29"/>
-      <c r="I71" s="32"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="31"/>
-      <c r="B72" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C72" s="29"/>
-      <c r="D72" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E72" s="30">
-        <v>42872</v>
-      </c>
-      <c r="F72" s="30"/>
-      <c r="G72" s="30"/>
-      <c r="H72" s="29"/>
-      <c r="I72" s="32"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="31"/>
-      <c r="B73" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E73" s="30">
-        <v>42872</v>
-      </c>
-      <c r="F73" s="30"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="30"/>
-      <c r="I73" s="32"/>
+      <c r="I62" s="27"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="31"/>
-      <c r="B74" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="C74" s="29"/>
-      <c r="D74" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E74" s="30">
-        <v>42872</v>
-      </c>
-      <c r="F74" s="30"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="33"/>
+      <c r="B74" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E74" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F74" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="G74" s="28"/>
+      <c r="H74" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="I74" s="32" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="31"/>
-      <c r="B75" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="C75" s="29"/>
-      <c r="D75" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E75" s="30">
-        <v>42872</v>
-      </c>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="29"/>
+      <c r="B75" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E75" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="27"/>
       <c r="I75" s="32"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="31"/>
-      <c r="B76" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="C76" s="29"/>
-      <c r="D76" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E76" s="30">
-        <v>42872</v>
-      </c>
-      <c r="F76" s="30"/>
-      <c r="G76" s="30"/>
-      <c r="H76" s="29"/>
+      <c r="B76" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E76" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F76" s="28"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="27"/>
       <c r="I76" s="32"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="31"/>
-      <c r="B77" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="C77" s="29"/>
-      <c r="D77" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E77" s="30">
-        <v>42873</v>
-      </c>
-      <c r="F77" s="29"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="29"/>
+      <c r="B77" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F77" s="28"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="27"/>
       <c r="I77" s="32"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="31"/>
-      <c r="B78" s="29" t="s">
+      <c r="B78" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E78" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F78" s="28"/>
+      <c r="G78" s="28"/>
+      <c r="H78" s="27"/>
+      <c r="I78" s="32"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="31"/>
+      <c r="B79" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E79" s="28">
+        <v>42870</v>
+      </c>
+      <c r="F79" s="28"/>
+      <c r="G79" s="28"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="32"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="31"/>
+      <c r="B80" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" s="27"/>
+      <c r="D80" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E80" s="30">
+        <v>42871</v>
+      </c>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="27"/>
+      <c r="I80" s="32"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="31"/>
+      <c r="B81" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="27"/>
+      <c r="D81" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E81" s="30">
+        <v>42871</v>
+      </c>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="32"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="31"/>
+      <c r="B82" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82" s="27"/>
+      <c r="D82" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E82" s="30">
+        <v>42871</v>
+      </c>
+      <c r="F82" s="28"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="27"/>
+      <c r="I82" s="32"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="31"/>
+      <c r="B83" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E83" s="30">
+        <v>42871</v>
+      </c>
+      <c r="F83" s="30"/>
+      <c r="G83" s="30"/>
+      <c r="H83" s="29"/>
+      <c r="I83" s="32"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="31"/>
+      <c r="B84" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E84" s="30">
+        <v>42871</v>
+      </c>
+      <c r="F84" s="30"/>
+      <c r="G84" s="30"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="32"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="31"/>
+      <c r="B85" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E85" s="30">
+        <v>42871</v>
+      </c>
+      <c r="F85" s="30"/>
+      <c r="G85" s="30"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="32"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="31"/>
+      <c r="B86" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E86" s="30">
+        <v>42871</v>
+      </c>
+      <c r="F86" s="30"/>
+      <c r="G86" s="30"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="32"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="31"/>
+      <c r="B87" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" s="30">
+        <v>42872</v>
+      </c>
+      <c r="F87" s="30"/>
+      <c r="G87" s="30"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="32"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="31"/>
+      <c r="B88" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88" s="30">
+        <v>42872</v>
+      </c>
+      <c r="F88" s="30"/>
+      <c r="G88" s="30"/>
+      <c r="H88" s="30"/>
+      <c r="I88" s="32"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="31"/>
+      <c r="B89" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E89" s="30">
+        <v>42872</v>
+      </c>
+      <c r="F89" s="30"/>
+      <c r="G89" s="30"/>
+      <c r="H89" s="30"/>
+      <c r="I89" s="33"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="31"/>
+      <c r="B90" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" s="30">
+        <v>42872</v>
+      </c>
+      <c r="F90" s="30"/>
+      <c r="G90" s="30"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="32"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="31"/>
+      <c r="B91" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E91" s="30">
+        <v>42872</v>
+      </c>
+      <c r="F91" s="30"/>
+      <c r="G91" s="30"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="32"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="31"/>
+      <c r="B92" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29" t="s">
+      <c r="C92" s="29"/>
+      <c r="D92" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="E78" s="30">
+      <c r="E92" s="30">
         <v>42873</v>
       </c>
-      <c r="F78" s="30"/>
-      <c r="G78" s="30"/>
-      <c r="H78" s="29"/>
-      <c r="I78" s="32"/>
-    </row>
-    <row r="79" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="34"/>
-      <c r="B79" s="35" t="s">
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="32"/>
+    </row>
+    <row r="93" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="31"/>
+      <c r="B93" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="C79" s="35"/>
-      <c r="D79" s="35" t="s">
+      <c r="C93" s="29"/>
+      <c r="D93" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E93" s="30">
+        <v>42873</v>
+      </c>
+      <c r="F93" s="30"/>
+      <c r="G93" s="30"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="32"/>
+    </row>
+    <row r="94" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="34"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="E79" s="36">
+      <c r="E94" s="36">
         <v>42874</v>
       </c>
-      <c r="F79" s="35"/>
-      <c r="G79" s="35"/>
-      <c r="H79" s="35"/>
-      <c r="I79" s="37"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
-      <c r="B81" s="15"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="35"/>
+      <c r="H94" s="35"/>
+      <c r="I94" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3481,10 +3639,10 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -3492,24 +3650,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" t="s">
         <v>240</v>
-      </c>
-      <c r="B4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C4" t="s">
-        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3533,51 +3691,51 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" s="66"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" s="66"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="65" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="66"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="65" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="66"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B7" s="66"/>
     </row>
     <row r="8" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8" s="68"/>
     </row>
@@ -3587,88 +3745,88 @@
     </row>
     <row r="10" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="75"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B11" s="64"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B12" s="66"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B13" s="66"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="65" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" s="66"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" s="66"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" s="66"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B19" s="66"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="65" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B20" s="66"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="65" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3677,16 +3835,16 @@
     </row>
     <row r="24" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B24" s="75"/>
     </row>
     <row r="25" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="69" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B25" s="70" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3699,42 +3857,42 @@
     </row>
     <row r="28" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B28" s="75"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B29" s="64"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="65" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30" s="66"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B32" s="66"/>
     </row>
     <row r="33" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B33" s="54" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3743,61 +3901,61 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B35" s="71"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B36" s="51"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B37" s="51"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B38" s="51"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B39" s="51"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B40" s="51"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B41" s="51"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B42" s="51"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B43" s="51"/>
     </row>
     <row r="44" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B44" s="54"/>
     </row>
@@ -3819,35 +3977,35 @@
     </row>
     <row r="49" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="77" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B49" s="75"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B50" s="71" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="65" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B52" s="51"/>
     </row>
     <row r="53" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="72" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B53" s="54"/>
     </row>
@@ -4057,7 +4215,7 @@
         <v>85</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>35</v>
@@ -4068,10 +4226,10 @@
         <v>42867</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>36</v>
@@ -4085,7 +4243,7 @@
         <v>85</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>37</v>
@@ -4099,7 +4257,7 @@
         <v>85</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Add a single space to test repo
</commit_message>
<xml_diff>
--- a/Proj 3 Plan.xlsx
+++ b/Proj 3 Plan.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="269">
   <si>
     <t>Technical Requirements</t>
   </si>
@@ -1068,6 +1068,9 @@
   </si>
   <si>
     <t>animation - optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -4562,10 +4565,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A42"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4573,80 +4576,83 @@
     <col min="1" max="1" width="108.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="83" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="81" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="79" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="79" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="79" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="79" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="79" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="72"/>
     </row>
-    <row r="10" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="82" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="78" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="79" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="79" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="79" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="79" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="79" t="s">
         <v>166</v>
       </c>

</xml_diff>